<commit_message>
get employee, upload leave files
</commit_message>
<xml_diff>
--- a/files/GDS-Leave-orders-from-Jan-2024.xlsx
+++ b/files/GDS-Leave-orders-from-Jan-2024.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mohankumar\projects-important\post-office-management-api\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E1F726B-4FCA-45B0-9671-82A567605794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAD231F-4C62-433B-A1E5-BA2354A34DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GDS-Leave-orders-from-Jan-2024" sheetId="1" r:id="rId1"/>
+    <sheet name="GDS Leave orders from Jan 2024" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="385">
-  <si>
-    <t>Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="398">
+  <si>
+    <t>SL.No</t>
   </si>
   <si>
     <t>Karthikeyan R</t>
@@ -1175,13 +1175,52 @@
   </si>
   <si>
     <t>Vijay</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>officeName</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>accountNo</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>substituteName</t>
+  </si>
+  <si>
+    <t>leaveType</t>
+  </si>
+  <si>
+    <t>postmanBeatNo</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>sendToHoOn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1312,12 +1351,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2021,66 +2054,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N283"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N283"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="22.109375" customWidth="1"/>
-    <col min="12" max="12" width="24.88671875" customWidth="1"/>
-    <col min="13" max="13" width="21.77734375" customWidth="1"/>
-    <col min="14" max="14" width="52.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="6" width="16.21875" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" customWidth="1"/>
+    <col min="10" max="10" width="20.21875" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" customWidth="1"/>
+    <col min="13" max="13" width="20.44140625" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>386</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>387</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>388</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>389</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="I1" t="s">
-        <v>0</v>
+        <v>391</v>
       </c>
       <c r="J1" t="s">
-        <v>0</v>
+        <v>392</v>
       </c>
       <c r="K1" t="s">
-        <v>0</v>
+        <v>394</v>
       </c>
       <c r="L1" t="s">
-        <v>0</v>
+        <v>395</v>
       </c>
       <c r="M1" t="s">
-        <v>0</v>
+        <v>396</v>
       </c>
       <c r="N1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -2121,7 +2164,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -2162,7 +2208,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -2176,7 +2225,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -2211,7 +2263,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -2246,7 +2301,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -2260,7 +2318,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -2295,7 +2356,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -2330,7 +2394,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -2365,7 +2432,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -2379,7 +2449,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -2393,7 +2466,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -2407,7 +2483,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -2445,7 +2524,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -2480,7 +2562,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -2515,7 +2600,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
       <c r="B17" t="s">
         <v>39</v>
       </c>
@@ -2550,7 +2638,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18" t="s">
         <v>39</v>
       </c>
@@ -2585,7 +2676,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="B19" t="s">
         <v>39</v>
       </c>
@@ -2620,7 +2714,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
         <v>39</v>
       </c>
@@ -2655,7 +2752,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="B21" t="s">
         <v>47</v>
       </c>
@@ -2669,7 +2769,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>49</v>
       </c>
@@ -2704,7 +2807,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
         <v>49</v>
       </c>
@@ -2739,7 +2845,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
       <c r="B24" t="s">
         <v>52</v>
       </c>
@@ -2774,7 +2883,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
       <c r="B25" t="s">
         <v>55</v>
       </c>
@@ -2788,7 +2900,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
       <c r="B26" t="s">
         <v>56</v>
       </c>
@@ -2823,7 +2938,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
       <c r="B27" t="s">
         <v>56</v>
       </c>
@@ -2858,7 +2976,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
       <c r="B28" t="s">
         <v>56</v>
       </c>
@@ -2893,7 +3014,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
       <c r="B29" t="s">
         <v>56</v>
       </c>
@@ -2928,7 +3052,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
       <c r="B30" t="s">
         <v>56</v>
       </c>
@@ -2963,7 +3090,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
       <c r="B31" t="s">
         <v>56</v>
       </c>
@@ -2998,7 +3128,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
       <c r="B32" t="s">
         <v>56</v>
       </c>
@@ -3033,7 +3166,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
       <c r="B33" t="s">
         <v>56</v>
       </c>
@@ -3068,7 +3204,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
       <c r="B34" t="s">
         <v>56</v>
       </c>
@@ -3103,7 +3242,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
       <c r="B35" t="s">
         <v>56</v>
       </c>
@@ -3138,7 +3280,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
       <c r="B36" t="s">
         <v>63</v>
       </c>
@@ -3173,7 +3318,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
       <c r="B37" t="s">
         <v>66</v>
       </c>
@@ -3187,7 +3335,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
       <c r="B38" t="s">
         <v>67</v>
       </c>
@@ -3201,7 +3352,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
       <c r="B39" t="s">
         <v>69</v>
       </c>
@@ -3215,7 +3369,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
       <c r="B40" t="s">
         <v>70</v>
       </c>
@@ -3256,7 +3413,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
       <c r="B41" t="s">
         <v>75</v>
       </c>
@@ -3291,7 +3451,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
       <c r="B42" t="s">
         <v>77</v>
       </c>
@@ -3326,7 +3489,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
       <c r="B43" t="s">
         <v>79</v>
       </c>
@@ -3361,7 +3527,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
       <c r="B44" t="s">
         <v>81</v>
       </c>
@@ -3375,7 +3544,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
       <c r="B45" t="s">
         <v>83</v>
       </c>
@@ -3389,7 +3561,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
       <c r="B46" t="s">
         <v>85</v>
       </c>
@@ -3403,7 +3578,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
       <c r="B47" t="s">
         <v>86</v>
       </c>
@@ -3438,7 +3616,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
       <c r="B48" t="s">
         <v>89</v>
       </c>
@@ -3473,7 +3654,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
       <c r="B49" t="s">
         <v>89</v>
       </c>
@@ -3508,7 +3692,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
       <c r="B50" t="s">
         <v>93</v>
       </c>
@@ -3543,7 +3730,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
       <c r="B51" t="s">
         <v>95</v>
       </c>
@@ -3578,7 +3768,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
       <c r="B52" t="s">
         <v>99</v>
       </c>
@@ -3592,7 +3785,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
       <c r="B53" t="s">
         <v>95</v>
       </c>
@@ -3627,7 +3823,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
       <c r="B54" t="s">
         <v>95</v>
       </c>
@@ -3662,7 +3861,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
       <c r="B55" t="s">
         <v>101</v>
       </c>
@@ -3676,7 +3878,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
       <c r="B56" t="s">
         <v>103</v>
       </c>
@@ -3711,7 +3916,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
       <c r="B57" t="s">
         <v>105</v>
       </c>
@@ -3746,7 +3954,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
       <c r="B58" t="s">
         <v>105</v>
       </c>
@@ -3781,7 +3992,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
       <c r="B59" t="s">
         <v>105</v>
       </c>
@@ -3816,7 +4030,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
       <c r="B60" t="s">
         <v>105</v>
       </c>
@@ -3851,7 +4068,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
       <c r="B61" t="s">
         <v>105</v>
       </c>
@@ -3886,7 +4106,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
       <c r="B62" t="s">
         <v>105</v>
       </c>
@@ -3921,7 +4144,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
       <c r="B63" t="s">
         <v>113</v>
       </c>
@@ -3959,7 +4185,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
       <c r="B64" t="s">
         <v>105</v>
       </c>
@@ -3994,7 +4223,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
       <c r="B65" t="s">
         <v>105</v>
       </c>
@@ -4029,7 +4261,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
       <c r="B66" t="s">
         <v>116</v>
       </c>
@@ -4064,7 +4299,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
       <c r="B67" t="s">
         <v>119</v>
       </c>
@@ -4099,7 +4337,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
       <c r="B68" t="s">
         <v>119</v>
       </c>
@@ -4134,7 +4375,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
       <c r="B69" t="s">
         <v>119</v>
       </c>
@@ -4169,7 +4413,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
       <c r="B70" t="s">
         <v>124</v>
       </c>
@@ -4183,7 +4430,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
       <c r="B71" t="s">
         <v>126</v>
       </c>
@@ -4218,7 +4468,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
       <c r="B72" t="s">
         <v>126</v>
       </c>
@@ -4253,7 +4506,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
       <c r="B73" t="s">
         <v>128</v>
       </c>
@@ -4267,7 +4523,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
       <c r="B74" t="s">
         <v>130</v>
       </c>
@@ -4281,7 +4540,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
       <c r="B75" t="s">
         <v>131</v>
       </c>
@@ -4316,7 +4578,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
       <c r="B76" t="s">
         <v>134</v>
       </c>
@@ -4351,7 +4616,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
       <c r="B77" t="s">
         <v>135</v>
       </c>
@@ -4386,7 +4654,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
       <c r="B78" t="s">
         <v>135</v>
       </c>
@@ -4421,7 +4692,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
       <c r="B79" t="s">
         <v>138</v>
       </c>
@@ -4435,7 +4709,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
       <c r="B80" t="s">
         <v>139</v>
       </c>
@@ -4449,7 +4726,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
       <c r="B81" t="s">
         <v>141</v>
       </c>
@@ -4484,7 +4764,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
       <c r="B82" t="s">
         <v>141</v>
       </c>
@@ -4519,7 +4802,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
       <c r="B83" t="s">
         <v>143</v>
       </c>
@@ -4554,7 +4840,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
       <c r="B84" t="s">
         <v>145</v>
       </c>
@@ -4589,7 +4878,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
       <c r="B85" t="s">
         <v>147</v>
       </c>
@@ -4603,7 +4895,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
       <c r="B86" t="s">
         <v>149</v>
       </c>
@@ -4617,7 +4912,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
       <c r="B87" t="s">
         <v>150</v>
       </c>
@@ -4631,7 +4929,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
       <c r="B88" t="s">
         <v>105</v>
       </c>
@@ -4666,7 +4967,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
       <c r="B89" t="s">
         <v>153</v>
       </c>
@@ -4683,7 +4987,10 @@
         <v>154</v>
       </c>
     </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
       <c r="B90" t="s">
         <v>155</v>
       </c>
@@ -4697,7 +5004,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
       <c r="B91" t="s">
         <v>157</v>
       </c>
@@ -4711,7 +5021,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
       <c r="B92" t="s">
         <v>158</v>
       </c>
@@ -4752,7 +5065,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
       <c r="B93" t="s">
         <v>158</v>
       </c>
@@ -4793,7 +5109,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
       <c r="B94" t="s">
         <v>163</v>
       </c>
@@ -4831,7 +5150,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
       <c r="B95" t="s">
         <v>165</v>
       </c>
@@ -4866,7 +5188,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
       <c r="B96" t="s">
         <v>167</v>
       </c>
@@ -4880,7 +5205,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
       <c r="B97" t="s">
         <v>169</v>
       </c>
@@ -4894,7 +5222,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
       <c r="B98" t="s">
         <v>170</v>
       </c>
@@ -4908,7 +5239,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
       <c r="B99" t="s">
         <v>172</v>
       </c>
@@ -4922,7 +5256,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
       <c r="B100" t="s">
         <v>173</v>
       </c>
@@ -4957,7 +5294,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>100</v>
+      </c>
       <c r="B101" t="s">
         <v>175</v>
       </c>
@@ -4971,7 +5311,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>101</v>
+      </c>
       <c r="B102" t="s">
         <v>176</v>
       </c>
@@ -4985,7 +5328,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>102</v>
+      </c>
       <c r="B103" t="s">
         <v>178</v>
       </c>
@@ -5026,7 +5372,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>103</v>
+      </c>
       <c r="B104" t="s">
         <v>178</v>
       </c>
@@ -5061,7 +5410,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>104</v>
+      </c>
       <c r="B105" t="s">
         <v>182</v>
       </c>
@@ -5096,7 +5448,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>105</v>
+      </c>
       <c r="B106" t="s">
         <v>182</v>
       </c>
@@ -5131,7 +5486,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>106</v>
+      </c>
       <c r="B107" t="s">
         <v>184</v>
       </c>
@@ -5166,7 +5524,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>107</v>
+      </c>
       <c r="B108" t="s">
         <v>186</v>
       </c>
@@ -5180,7 +5541,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>108</v>
+      </c>
       <c r="B109" t="s">
         <v>188</v>
       </c>
@@ -5221,7 +5585,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>109</v>
+      </c>
       <c r="B110" t="s">
         <v>188</v>
       </c>
@@ -5262,7 +5629,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>110</v>
+      </c>
       <c r="B111" t="s">
         <v>190</v>
       </c>
@@ -5297,7 +5667,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>111</v>
+      </c>
       <c r="B112" t="s">
         <v>190</v>
       </c>
@@ -5332,7 +5705,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>112</v>
+      </c>
       <c r="B113" t="s">
         <v>190</v>
       </c>
@@ -5367,7 +5743,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>113</v>
+      </c>
       <c r="B114" t="s">
         <v>190</v>
       </c>
@@ -5402,7 +5781,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>114</v>
+      </c>
       <c r="B115" t="s">
         <v>191</v>
       </c>
@@ -5437,7 +5819,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>115</v>
+      </c>
       <c r="B116" t="s">
         <v>193</v>
       </c>
@@ -5478,7 +5863,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>116</v>
+      </c>
       <c r="B117" t="s">
         <v>105</v>
       </c>
@@ -5513,7 +5901,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>117</v>
+      </c>
       <c r="B118" t="s">
         <v>196</v>
       </c>
@@ -5548,7 +5939,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>118</v>
+      </c>
       <c r="B119" t="s">
         <v>196</v>
       </c>
@@ -5583,7 +5977,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>119</v>
+      </c>
       <c r="B120" t="s">
         <v>200</v>
       </c>
@@ -5597,7 +5994,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>120</v>
+      </c>
       <c r="B121" t="s">
         <v>202</v>
       </c>
@@ -5632,7 +6032,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>121</v>
+      </c>
       <c r="B122" t="s">
         <v>202</v>
       </c>
@@ -5667,7 +6070,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>122</v>
+      </c>
       <c r="B123" t="s">
         <v>202</v>
       </c>
@@ -5702,7 +6108,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>123</v>
+      </c>
       <c r="B124" t="s">
         <v>202</v>
       </c>
@@ -5737,7 +6146,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>124</v>
+      </c>
       <c r="B125" t="s">
         <v>202</v>
       </c>
@@ -5772,7 +6184,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>125</v>
+      </c>
       <c r="B126" t="s">
         <v>202</v>
       </c>
@@ -5813,7 +6228,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>126</v>
+      </c>
       <c r="B127" t="s">
         <v>202</v>
       </c>
@@ -5848,7 +6266,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>127</v>
+      </c>
       <c r="B128" t="s">
         <v>205</v>
       </c>
@@ -5880,7 +6301,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>128</v>
+      </c>
       <c r="B129" t="s">
         <v>205</v>
       </c>
@@ -5915,7 +6339,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>129</v>
+      </c>
       <c r="B130" t="s">
         <v>208</v>
       </c>
@@ -5929,7 +6356,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>130</v>
+      </c>
       <c r="B131" t="s">
         <v>209</v>
       </c>
@@ -5964,7 +6394,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>131</v>
+      </c>
       <c r="B132" t="s">
         <v>105</v>
       </c>
@@ -6002,7 +6435,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>132</v>
+      </c>
       <c r="B133" t="s">
         <v>105</v>
       </c>
@@ -6037,7 +6473,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>133</v>
+      </c>
       <c r="B134" t="s">
         <v>105</v>
       </c>
@@ -6072,7 +6511,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>134</v>
+      </c>
       <c r="B135" t="s">
         <v>213</v>
       </c>
@@ -6107,7 +6549,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>135</v>
+      </c>
       <c r="B136" t="s">
         <v>216</v>
       </c>
@@ -6121,7 +6566,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>136</v>
+      </c>
       <c r="B137" t="s">
         <v>217</v>
       </c>
@@ -6156,7 +6604,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>137</v>
+      </c>
       <c r="B138" t="s">
         <v>219</v>
       </c>
@@ -6170,7 +6621,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>138</v>
+      </c>
       <c r="B139" t="s">
         <v>220</v>
       </c>
@@ -6184,7 +6638,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>139</v>
+      </c>
       <c r="B140" t="s">
         <v>222</v>
       </c>
@@ -6219,7 +6676,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="141" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>140</v>
+      </c>
       <c r="B141" t="s">
         <v>224</v>
       </c>
@@ -6254,7 +6714,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>141</v>
+      </c>
       <c r="B142" t="s">
         <v>224</v>
       </c>
@@ -6289,7 +6752,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>142</v>
+      </c>
       <c r="B143" t="s">
         <v>226</v>
       </c>
@@ -6324,7 +6790,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>143</v>
+      </c>
       <c r="B144" t="s">
         <v>228</v>
       </c>
@@ -6359,7 +6828,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>144</v>
+      </c>
       <c r="B145" t="s">
         <v>105</v>
       </c>
@@ -6394,7 +6866,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>145</v>
+      </c>
       <c r="B146" t="s">
         <v>105</v>
       </c>
@@ -6429,7 +6904,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>146</v>
+      </c>
       <c r="B147" t="s">
         <v>105</v>
       </c>
@@ -6464,7 +6942,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>147</v>
+      </c>
       <c r="B148" t="s">
         <v>105</v>
       </c>
@@ -6499,7 +6980,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>148</v>
+      </c>
       <c r="B149" t="s">
         <v>232</v>
       </c>
@@ -6534,7 +7018,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>149</v>
+      </c>
       <c r="B150" t="s">
         <v>232</v>
       </c>
@@ -6569,7 +7056,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>150</v>
+      </c>
       <c r="B151" t="s">
         <v>232</v>
       </c>
@@ -6610,7 +7100,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>151</v>
+      </c>
       <c r="B152" t="s">
         <v>232</v>
       </c>
@@ -6651,7 +7144,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>152</v>
+      </c>
       <c r="B153" t="s">
         <v>163</v>
       </c>
@@ -6689,7 +7185,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>153</v>
+      </c>
       <c r="B154" t="s">
         <v>236</v>
       </c>
@@ -6700,7 +7199,10 @@
         <v>233</v>
       </c>
     </row>
-    <row r="155" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>154</v>
+      </c>
       <c r="B155" t="s">
         <v>237</v>
       </c>
@@ -6714,7 +7216,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>155</v>
+      </c>
       <c r="B156" t="s">
         <v>238</v>
       </c>
@@ -6728,7 +7233,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>156</v>
+      </c>
       <c r="B157" t="s">
         <v>105</v>
       </c>
@@ -6766,7 +7274,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>157</v>
+      </c>
       <c r="B158" t="s">
         <v>105</v>
       </c>
@@ -6801,7 +7312,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>158</v>
+      </c>
       <c r="B159" t="s">
         <v>241</v>
       </c>
@@ -6836,7 +7350,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>159</v>
+      </c>
       <c r="B160" t="s">
         <v>241</v>
       </c>
@@ -6871,7 +7388,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>160</v>
+      </c>
       <c r="B161" t="s">
         <v>105</v>
       </c>
@@ -6906,7 +7426,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>161</v>
+      </c>
       <c r="B162" t="s">
         <v>243</v>
       </c>
@@ -6941,7 +7464,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>162</v>
+      </c>
       <c r="B163" t="s">
         <v>243</v>
       </c>
@@ -6976,7 +7502,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>163</v>
+      </c>
       <c r="B164" t="s">
         <v>245</v>
       </c>
@@ -7011,7 +7540,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>164</v>
+      </c>
       <c r="B165" t="s">
         <v>247</v>
       </c>
@@ -7028,7 +7560,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>165</v>
+      </c>
       <c r="B166" t="s">
         <v>249</v>
       </c>
@@ -7063,7 +7598,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>166</v>
+      </c>
       <c r="B167" t="s">
         <v>249</v>
       </c>
@@ -7098,7 +7636,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>167</v>
+      </c>
       <c r="B168" t="s">
         <v>249</v>
       </c>
@@ -7133,7 +7674,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>168</v>
+      </c>
       <c r="B169" t="s">
         <v>251</v>
       </c>
@@ -7168,7 +7712,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>169</v>
+      </c>
       <c r="B170" t="s">
         <v>251</v>
       </c>
@@ -7203,7 +7750,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>170</v>
+      </c>
       <c r="B171" t="s">
         <v>253</v>
       </c>
@@ -7238,7 +7788,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="172" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>171</v>
+      </c>
       <c r="B172" t="s">
         <v>254</v>
       </c>
@@ -7252,7 +7805,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>172</v>
+      </c>
       <c r="B173" t="s">
         <v>256</v>
       </c>
@@ -7287,7 +7843,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>173</v>
+      </c>
       <c r="B174" t="s">
         <v>256</v>
       </c>
@@ -7322,7 +7881,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>174</v>
+      </c>
       <c r="B175" t="s">
         <v>258</v>
       </c>
@@ -7357,7 +7919,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>175</v>
+      </c>
       <c r="B176" t="s">
         <v>260</v>
       </c>
@@ -7392,7 +7957,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>176</v>
+      </c>
       <c r="B177" t="s">
         <v>262</v>
       </c>
@@ -7427,7 +7995,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="178" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>177</v>
+      </c>
       <c r="B178" t="s">
         <v>262</v>
       </c>
@@ -7462,7 +8033,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>178</v>
+      </c>
       <c r="B179" t="s">
         <v>265</v>
       </c>
@@ -7476,7 +8050,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>179</v>
+      </c>
       <c r="B180" t="s">
         <v>267</v>
       </c>
@@ -7490,7 +8067,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>180</v>
+      </c>
       <c r="B181" t="s">
         <v>268</v>
       </c>
@@ -7525,7 +8105,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>181</v>
+      </c>
       <c r="B182" t="s">
         <v>268</v>
       </c>
@@ -7560,7 +8143,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>182</v>
+      </c>
       <c r="B183" t="s">
         <v>272</v>
       </c>
@@ -7601,7 +8187,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>183</v>
+      </c>
       <c r="B184" t="s">
         <v>272</v>
       </c>
@@ -7642,7 +8231,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>184</v>
+      </c>
       <c r="B185" t="s">
         <v>272</v>
       </c>
@@ -7683,7 +8275,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>185</v>
+      </c>
       <c r="B186" t="s">
         <v>272</v>
       </c>
@@ -7718,7 +8313,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>186</v>
+      </c>
       <c r="B187" t="s">
         <v>272</v>
       </c>
@@ -7759,7 +8357,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>187</v>
+      </c>
       <c r="B188" t="s">
         <v>275</v>
       </c>
@@ -7794,7 +8395,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>188</v>
+      </c>
       <c r="B189" t="s">
         <v>275</v>
       </c>
@@ -7829,7 +8433,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>189</v>
+      </c>
       <c r="B190" t="s">
         <v>277</v>
       </c>
@@ -7864,7 +8471,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="191" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>190</v>
+      </c>
       <c r="B191" t="s">
         <v>279</v>
       </c>
@@ -7899,7 +8509,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>191</v>
+      </c>
       <c r="B192" t="s">
         <v>281</v>
       </c>
@@ -7913,7 +8526,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>192</v>
+      </c>
       <c r="B193" t="s">
         <v>283</v>
       </c>
@@ -7927,7 +8543,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>193</v>
+      </c>
       <c r="B194" t="s">
         <v>284</v>
       </c>
@@ -7941,7 +8560,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>194</v>
+      </c>
       <c r="B195" t="s">
         <v>105</v>
       </c>
@@ -7976,7 +8598,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>195</v>
+      </c>
       <c r="B196" t="s">
         <v>105</v>
       </c>
@@ -8011,7 +8636,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>196</v>
+      </c>
       <c r="B197" t="s">
         <v>105</v>
       </c>
@@ -8049,7 +8677,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>197</v>
+      </c>
       <c r="B198" t="s">
         <v>288</v>
       </c>
@@ -8063,7 +8694,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>198</v>
+      </c>
       <c r="B199" t="s">
         <v>290</v>
       </c>
@@ -8098,7 +8732,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="200" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>199</v>
+      </c>
       <c r="B200" t="s">
         <v>290</v>
       </c>
@@ -8133,7 +8770,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>200</v>
+      </c>
       <c r="B201" t="s">
         <v>290</v>
       </c>
@@ -8168,7 +8808,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>201</v>
+      </c>
       <c r="B202" t="s">
         <v>290</v>
       </c>
@@ -8203,7 +8846,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>202</v>
+      </c>
       <c r="B203" t="s">
         <v>292</v>
       </c>
@@ -8238,7 +8884,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>203</v>
+      </c>
       <c r="B204" t="s">
         <v>294</v>
       </c>
@@ -8252,7 +8901,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>204</v>
+      </c>
       <c r="B205" t="s">
         <v>295</v>
       </c>
@@ -8266,7 +8918,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>205</v>
+      </c>
       <c r="B206" t="s">
         <v>297</v>
       </c>
@@ -8280,7 +8935,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>206</v>
+      </c>
       <c r="B207" t="s">
         <v>298</v>
       </c>
@@ -8294,7 +8952,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>207</v>
+      </c>
       <c r="B208" t="s">
         <v>300</v>
       </c>
@@ -8308,7 +8969,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>208</v>
+      </c>
       <c r="B209" t="s">
         <v>163</v>
       </c>
@@ -8346,7 +9010,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>209</v>
+      </c>
       <c r="B210" t="s">
         <v>303</v>
       </c>
@@ -8381,7 +9048,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>210</v>
+      </c>
       <c r="B211" t="s">
         <v>303</v>
       </c>
@@ -8416,7 +9086,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="212" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>211</v>
+      </c>
       <c r="B212" t="s">
         <v>306</v>
       </c>
@@ -8451,7 +9124,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>212</v>
+      </c>
       <c r="B213" t="s">
         <v>306</v>
       </c>
@@ -8486,7 +9162,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A214">
+        <v>213</v>
+      </c>
       <c r="B214" t="s">
         <v>306</v>
       </c>
@@ -8521,7 +9200,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A215">
+        <v>214</v>
+      </c>
       <c r="B215" t="s">
         <v>306</v>
       </c>
@@ -8556,7 +9238,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A216">
+        <v>215</v>
+      </c>
       <c r="B216" t="s">
         <v>308</v>
       </c>
@@ -8591,7 +9276,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="217" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>216</v>
+      </c>
       <c r="B217" t="s">
         <v>310</v>
       </c>
@@ -8605,7 +9293,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>217</v>
+      </c>
       <c r="B218" t="s">
         <v>311</v>
       </c>
@@ -8619,7 +9310,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>218</v>
+      </c>
       <c r="B219" t="s">
         <v>313</v>
       </c>
@@ -8654,7 +9348,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>219</v>
+      </c>
       <c r="B220" t="s">
         <v>313</v>
       </c>
@@ -8689,7 +9386,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>220</v>
+      </c>
       <c r="B221" t="s">
         <v>316</v>
       </c>
@@ -8703,7 +9403,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>221</v>
+      </c>
       <c r="B222" t="s">
         <v>318</v>
       </c>
@@ -8744,7 +9447,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="223" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A223">
+        <v>222</v>
+      </c>
       <c r="B223" t="s">
         <v>318</v>
       </c>
@@ -8785,7 +9491,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="224" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A224">
+        <v>223</v>
+      </c>
       <c r="B224" t="s">
         <v>318</v>
       </c>
@@ -8826,7 +9535,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A225">
+        <v>224</v>
+      </c>
       <c r="B225" t="s">
         <v>318</v>
       </c>
@@ -8867,7 +9579,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="226" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A226">
+        <v>225</v>
+      </c>
       <c r="B226" t="s">
         <v>318</v>
       </c>
@@ -8908,7 +9623,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="227" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>226</v>
+      </c>
       <c r="B227" t="s">
         <v>320</v>
       </c>
@@ -8922,7 +9640,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A228">
+        <v>227</v>
+      </c>
       <c r="B228" t="s">
         <v>105</v>
       </c>
@@ -8960,7 +9681,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A229">
+        <v>228</v>
+      </c>
       <c r="B229" t="s">
         <v>326</v>
       </c>
@@ -8995,7 +9719,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>229</v>
+      </c>
       <c r="B230" t="s">
         <v>328</v>
       </c>
@@ -9009,7 +9736,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>230</v>
+      </c>
       <c r="B231" t="s">
         <v>222</v>
       </c>
@@ -9023,7 +9753,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>231</v>
+      </c>
       <c r="B232" t="s">
         <v>330</v>
       </c>
@@ -9058,7 +9791,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>232</v>
+      </c>
       <c r="B233" t="s">
         <v>105</v>
       </c>
@@ -9093,7 +9829,10 @@
         <v>45293</v>
       </c>
     </row>
-    <row r="234" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>233</v>
+      </c>
       <c r="B234" t="s">
         <v>334</v>
       </c>
@@ -9128,7 +9867,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="235" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>234</v>
+      </c>
       <c r="B235" t="s">
         <v>105</v>
       </c>
@@ -9163,7 +9905,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>235</v>
+      </c>
       <c r="B236" t="s">
         <v>337</v>
       </c>
@@ -9198,7 +9943,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>236</v>
+      </c>
       <c r="B237" t="s">
         <v>337</v>
       </c>
@@ -9233,7 +9981,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="238" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>237</v>
+      </c>
       <c r="B238" t="s">
         <v>337</v>
       </c>
@@ -9268,7 +10019,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="239" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>238</v>
+      </c>
       <c r="B239" t="s">
         <v>341</v>
       </c>
@@ -9303,7 +10057,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>239</v>
+      </c>
       <c r="B240" t="s">
         <v>343</v>
       </c>
@@ -9338,7 +10095,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="241" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>240</v>
+      </c>
       <c r="B241" t="s">
         <v>344</v>
       </c>
@@ -9373,7 +10133,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>241</v>
+      </c>
       <c r="B242" t="s">
         <v>345</v>
       </c>
@@ -9408,7 +10171,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>242</v>
+      </c>
       <c r="B243" t="s">
         <v>347</v>
       </c>
@@ -9443,7 +10209,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="244" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>243</v>
+      </c>
       <c r="B244" t="s">
         <v>347</v>
       </c>
@@ -9478,7 +10247,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>244</v>
+      </c>
       <c r="B245" t="s">
         <v>350</v>
       </c>
@@ -9513,7 +10285,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>245</v>
+      </c>
       <c r="B246" t="s">
         <v>351</v>
       </c>
@@ -9548,7 +10323,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="247" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>246</v>
+      </c>
       <c r="B247" t="s">
         <v>354</v>
       </c>
@@ -9583,7 +10361,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>247</v>
+      </c>
       <c r="B248" t="s">
         <v>354</v>
       </c>
@@ -9618,7 +10399,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="249" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>248</v>
+      </c>
       <c r="B249" t="s">
         <v>356</v>
       </c>
@@ -9653,7 +10437,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>249</v>
+      </c>
       <c r="B250" t="s">
         <v>356</v>
       </c>
@@ -9688,7 +10475,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="251" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>250</v>
+      </c>
       <c r="B251" t="s">
         <v>356</v>
       </c>
@@ -9726,7 +10516,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="252" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>251</v>
+      </c>
       <c r="B252" t="s">
         <v>359</v>
       </c>
@@ -9761,7 +10554,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="253" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>252</v>
+      </c>
       <c r="B253" t="s">
         <v>360</v>
       </c>
@@ -9796,7 +10592,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="254" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>253</v>
+      </c>
       <c r="B254" t="s">
         <v>360</v>
       </c>
@@ -9831,7 +10630,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="255" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>254</v>
+      </c>
       <c r="B255" t="s">
         <v>361</v>
       </c>
@@ -9866,7 +10668,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>255</v>
+      </c>
       <c r="B256" t="s">
         <v>361</v>
       </c>
@@ -9901,7 +10706,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="257" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>256</v>
+      </c>
       <c r="B257" t="s">
         <v>361</v>
       </c>
@@ -9936,7 +10744,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>257</v>
+      </c>
       <c r="B258" t="s">
         <v>361</v>
       </c>
@@ -9971,7 +10782,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="259" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>258</v>
+      </c>
       <c r="B259" t="s">
         <v>361</v>
       </c>
@@ -10012,7 +10826,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>259</v>
+      </c>
       <c r="B260" t="s">
         <v>361</v>
       </c>
@@ -10053,7 +10870,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>260</v>
+      </c>
       <c r="B261" t="s">
         <v>361</v>
       </c>
@@ -10094,7 +10914,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="262" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>261</v>
+      </c>
       <c r="B262" t="s">
         <v>363</v>
       </c>
@@ -10129,7 +10952,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>262</v>
+      </c>
       <c r="B263" t="s">
         <v>363</v>
       </c>
@@ -10164,7 +10990,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="264" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>263</v>
+      </c>
       <c r="B264" t="s">
         <v>363</v>
       </c>
@@ -10199,7 +11028,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="265" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>264</v>
+      </c>
       <c r="B265" t="s">
         <v>364</v>
       </c>
@@ -10240,7 +11072,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="266" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>265</v>
+      </c>
       <c r="B266" t="s">
         <v>364</v>
       </c>
@@ -10281,7 +11116,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="267" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>266</v>
+      </c>
       <c r="B267" t="s">
         <v>369</v>
       </c>
@@ -10322,7 +11160,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="268" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>267</v>
+      </c>
       <c r="B268" t="s">
         <v>369</v>
       </c>
@@ -10363,7 +11204,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="269" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>268</v>
+      </c>
       <c r="B269" t="s">
         <v>369</v>
       </c>
@@ -10398,7 +11242,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="270" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>269</v>
+      </c>
       <c r="B270" t="s">
         <v>369</v>
       </c>
@@ -10433,7 +11280,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="271" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>270</v>
+      </c>
       <c r="B271" t="s">
         <v>105</v>
       </c>
@@ -10468,7 +11318,10 @@
         <v>45293</v>
       </c>
     </row>
-    <row r="272" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>271</v>
+      </c>
       <c r="B272" t="s">
         <v>105</v>
       </c>
@@ -10506,7 +11359,10 @@
         <v>45293</v>
       </c>
     </row>
-    <row r="273" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>272</v>
+      </c>
       <c r="B273" t="s">
         <v>373</v>
       </c>
@@ -10547,7 +11403,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>273</v>
+      </c>
       <c r="B274" t="s">
         <v>376</v>
       </c>
@@ -10588,7 +11447,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="275" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A275">
+        <v>274</v>
+      </c>
       <c r="B275" t="s">
         <v>376</v>
       </c>
@@ -10629,7 +11491,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="276" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A276">
+        <v>275</v>
+      </c>
       <c r="B276" t="s">
         <v>377</v>
       </c>
@@ -10643,7 +11508,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A277">
+        <v>276</v>
+      </c>
       <c r="B277" t="s">
         <v>379</v>
       </c>
@@ -10681,7 +11549,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A278">
+        <v>277</v>
+      </c>
       <c r="B278" t="s">
         <v>379</v>
       </c>
@@ -10716,7 +11587,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A279">
+        <v>278</v>
+      </c>
       <c r="B279" t="s">
         <v>379</v>
       </c>
@@ -10754,7 +11628,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="280" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A280">
+        <v>279</v>
+      </c>
       <c r="B280" t="s">
         <v>379</v>
       </c>
@@ -10789,7 +11666,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="281" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A281">
+        <v>280</v>
+      </c>
       <c r="B281" t="s">
         <v>379</v>
       </c>
@@ -10824,7 +11704,10 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="282" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A282">
+        <v>281</v>
+      </c>
       <c r="B282" t="s">
         <v>381</v>
       </c>
@@ -10859,7 +11742,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A283">
+        <v>282</v>
+      </c>
       <c r="B283" t="s">
         <v>384</v>
       </c>
@@ -10874,7 +11760,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>